<commit_message>
hapus kolom sudah pengumuman dan nomor pengumuman
</commit_message>
<xml_diff>
--- a/public/Nominatif Pendaftaran PTSL Desa Pondokjoyo.xlsx
+++ b/public/Nominatif Pendaftaran PTSL Desa Pondokjoyo.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="99">
   <si>
     <t>No Nominatif</t>
   </si>
@@ -29,12 +29,6 @@
     <t>No Pengumuman</t>
   </si>
   <si>
-    <t>Sudah Pengumuman</t>
-  </si>
-  <si>
-    <t>Tanggal Pendataan</t>
-  </si>
-  <si>
     <t>PBT</t>
   </si>
   <si>
@@ -242,10 +236,10 @@
     <t>0011</t>
   </si>
   <si>
-    <t>2314/2023</t>
-  </si>
-  <si>
-    <t>90%</t>
+    <t>012345</t>
+  </si>
+  <si>
+    <t>10%</t>
   </si>
   <si>
     <t>3509072008000002</t>
@@ -266,7 +260,7 @@
     <t>ISLAM</t>
   </si>
   <si>
-    <t>WIRASWASTA</t>
+    <t>MAHASISWA</t>
   </si>
   <si>
     <t>002</t>
@@ -275,7 +269,7 @@
     <t>003</t>
   </si>
   <si>
-    <t>BETENG</t>
+    <t>SONGON</t>
   </si>
   <si>
     <t>PONDOKJOYO</t>
@@ -293,55 +287,31 @@
     <t>PEKARANGAN</t>
   </si>
   <si>
-    <t>UTARA</t>
-  </si>
-  <si>
-    <t>TIMUR</t>
-  </si>
-  <si>
-    <t>SELATAN</t>
-  </si>
-  <si>
-    <t>BARAT</t>
-  </si>
-  <si>
-    <t>AMIRA</t>
-  </si>
-  <si>
-    <t>JUAL BELI</t>
-  </si>
-  <si>
-    <t>BELI 1</t>
+    <t>JALAN DESA</t>
+  </si>
+  <si>
+    <t>TANAH ORANG</t>
+  </si>
+  <si>
+    <t>ORANG 1</t>
+  </si>
+  <si>
+    <t>ORANG 2</t>
   </si>
   <si>
     <t>WARIS</t>
   </si>
   <si>
-    <t>WARISAN INI BOS</t>
+    <t>WARIS 2</t>
+  </si>
+  <si>
+    <t>JUAL BELI 3</t>
   </si>
   <si>
     <t>DIDIK SAENULLA</t>
   </si>
   <si>
-    <t>ABAS SAI'UL ULUM</t>
-  </si>
-  <si>
-    <t>3509072009000002</t>
-  </si>
-  <si>
-    <t>drajad 1</t>
-  </si>
-  <si>
-    <t>drajad 2</t>
-  </si>
-  <si>
-    <t>HIBAH</t>
-  </si>
-  <si>
-    <t>hibah ini</t>
-  </si>
-  <si>
-    <t>jual beli akhir</t>
+    <t>EDI BEDOR</t>
   </si>
 </sst>
 </file>
@@ -677,7 +647,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:BU3"/>
+  <dimension ref="A1:BS2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -685,7 +655,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:73">
+    <row r="1" spans="1:71">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -899,43 +869,41 @@
       <c r="BS1" t="s">
         <v>70</v>
       </c>
-      <c r="BT1" t="s">
+    </row>
+    <row r="2" spans="1:71">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
         <v>71</v>
       </c>
-      <c r="BU1" t="s">
+      <c r="C2" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="2" spans="1:73">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="D2"/>
+      <c r="E2">
+        <v>12345</v>
+      </c>
+      <c r="F2">
+        <v>12345</v>
+      </c>
+      <c r="G2">
+        <v>11.22</v>
+      </c>
+      <c r="H2" t="s">
         <v>73</v>
       </c>
-      <c r="C2" t="s">
+      <c r="I2">
+        <v>1000</v>
+      </c>
+      <c r="J2">
+        <v>100</v>
+      </c>
+      <c r="K2" t="s">
         <v>74</v>
       </c>
-      <c r="D2"/>
-      <c r="E2"/>
-      <c r="F2"/>
-      <c r="G2" t="s">
+      <c r="L2" t="s">
         <v>75</v>
-      </c>
-      <c r="H2">
-        <v>145678</v>
-      </c>
-      <c r="I2">
-        <v>11.11</v>
-      </c>
-      <c r="J2">
-        <v>123456</v>
-      </c>
-      <c r="K2">
-        <v>1000</v>
-      </c>
-      <c r="L2">
-        <v>900</v>
       </c>
       <c r="M2" t="s">
         <v>76</v>
@@ -946,23 +914,23 @@
       <c r="O2" t="s">
         <v>78</v>
       </c>
-      <c r="P2" t="s">
+      <c r="P2">
+        <v>22</v>
+      </c>
+      <c r="Q2" t="s">
         <v>79</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>80</v>
-      </c>
-      <c r="R2">
-        <v>22</v>
       </c>
       <c r="S2" t="s">
         <v>81</v>
       </c>
       <c r="T2" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="U2" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="V2" t="s">
         <v>77</v>
@@ -970,17 +938,17 @@
       <c r="W2" t="s">
         <v>78</v>
       </c>
-      <c r="X2" t="s">
+      <c r="X2">
+        <v>22</v>
+      </c>
+      <c r="Y2" t="s">
         <v>79</v>
       </c>
-      <c r="Y2" t="s">
-        <v>80</v>
-      </c>
-      <c r="Z2">
-        <v>22</v>
+      <c r="Z2" t="s">
+        <v>82</v>
       </c>
       <c r="AA2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="AB2" t="s">
         <v>84</v>
@@ -991,88 +959,82 @@
       <c r="AD2" t="s">
         <v>86</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AE2">
+        <v>2000</v>
+      </c>
+      <c r="AF2">
+        <v>12345</v>
+      </c>
+      <c r="AG2">
+        <v>12345</v>
+      </c>
+      <c r="AH2" t="s">
         <v>87</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AI2" t="s">
         <v>88</v>
-      </c>
-      <c r="AG2">
-        <v>1960</v>
-      </c>
-      <c r="AH2">
-        <v>3456</v>
-      </c>
-      <c r="AI2">
-        <v>345</v>
       </c>
       <c r="AJ2" t="s">
         <v>89</v>
       </c>
-      <c r="AK2" t="s">
+      <c r="AK2">
+        <v>900</v>
+      </c>
+      <c r="AL2" t="s">
         <v>90</v>
       </c>
-      <c r="AL2" t="s">
+      <c r="AM2" t="s">
         <v>91</v>
       </c>
-      <c r="AM2">
-        <v>100</v>
-      </c>
       <c r="AN2" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>90</v>
+      </c>
+      <c r="AP2">
+        <v>2000</v>
+      </c>
+      <c r="AQ2" t="s">
         <v>92</v>
       </c>
-      <c r="AO2" t="s">
+      <c r="AR2">
+        <v>2010</v>
+      </c>
+      <c r="AS2" t="s">
         <v>93</v>
       </c>
-      <c r="AP2" t="s">
+      <c r="AT2" t="s">
         <v>94</v>
       </c>
-      <c r="AQ2" t="s">
+      <c r="AU2" t="s">
         <v>95</v>
       </c>
-      <c r="AR2">
-        <v>1960</v>
-      </c>
-      <c r="AS2" t="s">
-        <v>78</v>
-      </c>
-      <c r="AT2">
-        <v>2000</v>
-      </c>
-      <c r="AU2" t="s">
+      <c r="AV2" t="s">
+        <v>93</v>
+      </c>
+      <c r="AW2">
+        <v>2023</v>
+      </c>
+      <c r="AX2"/>
+      <c r="AY2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AZ2"/>
+      <c r="BA2"/>
+      <c r="BB2"/>
+      <c r="BC2" t="s">
         <v>96</v>
       </c>
-      <c r="AV2" t="s">
+      <c r="BD2"/>
+      <c r="BE2" t="s">
+        <v>96</v>
+      </c>
+      <c r="BF2" t="s">
         <v>97</v>
       </c>
-      <c r="AW2" t="s">
-        <v>98</v>
-      </c>
-      <c r="AX2" t="s">
-        <v>96</v>
-      </c>
-      <c r="AY2">
-        <v>2022</v>
-      </c>
-      <c r="AZ2" t="s">
-        <v>99</v>
-      </c>
-      <c r="BA2" t="s">
-        <v>78</v>
-      </c>
-      <c r="BB2"/>
-      <c r="BC2"/>
-      <c r="BD2" t="s">
-        <v>100</v>
-      </c>
-      <c r="BE2"/>
-      <c r="BF2"/>
-      <c r="BG2" t="s">
-        <v>100</v>
-      </c>
-      <c r="BH2" t="s">
-        <v>101</v>
-      </c>
+      <c r="BG2"/>
+      <c r="BH2"/>
       <c r="BI2"/>
       <c r="BJ2"/>
       <c r="BK2"/>
@@ -1083,137 +1045,8 @@
       <c r="BP2"/>
       <c r="BQ2"/>
       <c r="BR2"/>
-      <c r="BS2"/>
-      <c r="BT2"/>
-      <c r="BU2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="3" spans="1:73">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3"/>
-      <c r="C3"/>
-      <c r="D3"/>
-      <c r="E3"/>
-      <c r="F3"/>
-      <c r="G3"/>
-      <c r="H3"/>
-      <c r="I3"/>
-      <c r="J3"/>
-      <c r="K3"/>
-      <c r="L3">
-        <v>0</v>
-      </c>
-      <c r="M3"/>
-      <c r="N3" t="s">
-        <v>103</v>
-      </c>
-      <c r="O3" t="s">
-        <v>78</v>
-      </c>
-      <c r="P3"/>
-      <c r="Q3"/>
-      <c r="R3"/>
-      <c r="S3"/>
-      <c r="T3" t="s">
-        <v>82</v>
-      </c>
-      <c r="U3"/>
-      <c r="V3" t="s">
-        <v>103</v>
-      </c>
-      <c r="W3" t="s">
-        <v>78</v>
-      </c>
-      <c r="X3"/>
-      <c r="Y3"/>
-      <c r="Z3"/>
-      <c r="AA3"/>
-      <c r="AB3"/>
-      <c r="AC3"/>
-      <c r="AD3"/>
-      <c r="AE3" t="s">
-        <v>87</v>
-      </c>
-      <c r="AF3" t="s">
-        <v>88</v>
-      </c>
-      <c r="AG3">
-        <v>1960</v>
-      </c>
-      <c r="AH3"/>
-      <c r="AI3"/>
-      <c r="AJ3"/>
-      <c r="AK3" t="s">
-        <v>90</v>
-      </c>
-      <c r="AL3" t="s">
-        <v>91</v>
-      </c>
-      <c r="AM3"/>
-      <c r="AN3"/>
-      <c r="AO3"/>
-      <c r="AP3"/>
-      <c r="AQ3"/>
-      <c r="AR3">
-        <v>1960</v>
-      </c>
-      <c r="AS3" t="s">
-        <v>104</v>
-      </c>
-      <c r="AT3">
-        <v>2000</v>
-      </c>
-      <c r="AU3" t="s">
-        <v>105</v>
-      </c>
-      <c r="AV3" t="s">
-        <v>106</v>
-      </c>
-      <c r="AW3" t="s">
-        <v>107</v>
-      </c>
-      <c r="AX3" t="s">
-        <v>105</v>
-      </c>
-      <c r="AY3">
-        <v>2022</v>
-      </c>
-      <c r="AZ3" t="s">
-        <v>97</v>
-      </c>
-      <c r="BA3" t="s">
-        <v>78</v>
-      </c>
-      <c r="BB3"/>
-      <c r="BC3"/>
-      <c r="BD3"/>
-      <c r="BE3" t="s">
-        <v>108</v>
-      </c>
-      <c r="BF3"/>
-      <c r="BG3" t="s">
-        <v>108</v>
-      </c>
-      <c r="BH3" t="s">
-        <v>101</v>
-      </c>
-      <c r="BI3"/>
-      <c r="BJ3"/>
-      <c r="BK3"/>
-      <c r="BL3"/>
-      <c r="BM3"/>
-      <c r="BN3"/>
-      <c r="BO3"/>
-      <c r="BP3"/>
-      <c r="BQ3"/>
-      <c r="BR3"/>
-      <c r="BS3"/>
-      <c r="BT3"/>
-      <c r="BU3" t="s">
-        <v>102</v>
+      <c r="BS2" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
atur tanggal format dd-mm-yyyy
</commit_message>
<xml_diff>
--- a/public/Nominatif Pendaftaran PTSL Desa Pondokjoyo.xlsx
+++ b/public/Nominatif Pendaftaran PTSL Desa Pondokjoyo.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="100">
   <si>
     <t>No Nominatif</t>
   </si>
@@ -26,7 +26,7 @@
     <t>No SPPT</t>
   </si>
   <si>
-    <t>No Pengumuman</t>
+    <t>Tanggal Pendataan</t>
   </si>
   <si>
     <t>PBT</t>
@@ -236,6 +236,9 @@
     <t>0011</t>
   </si>
   <si>
+    <t>11-02-2023</t>
+  </si>
+  <si>
     <t>012345</t>
   </si>
   <si>
@@ -251,7 +254,7 @@
     <t>JEMBER</t>
   </si>
   <si>
-    <t>2000-08-20</t>
+    <t>20-08-2000</t>
   </si>
   <si>
     <t>JALAN BENDO GANG 3 NO. 36 DESA SIDOMEKAR KECAMATAN SEMBORO</t>
@@ -272,7 +275,7 @@
     <t>SONGON</t>
   </si>
   <si>
-    <t>PONDOKJOYO</t>
+    <t>PONDOK JOYO</t>
   </si>
   <si>
     <t>SEMBORO</t>
@@ -880,7 +883,9 @@
       <c r="C2" t="s">
         <v>72</v>
       </c>
-      <c r="D2"/>
+      <c r="D2" t="s">
+        <v>73</v>
+      </c>
       <c r="E2">
         <v>12345</v>
       </c>
@@ -891,7 +896,7 @@
         <v>11.22</v>
       </c>
       <c r="H2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="I2">
         <v>1000</v>
@@ -900,64 +905,64 @@
         <v>100</v>
       </c>
       <c r="K2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="L2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="M2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="N2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="O2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="P2">
         <v>22</v>
       </c>
       <c r="Q2" t="s">
+        <v>80</v>
+      </c>
+      <c r="R2" t="s">
+        <v>81</v>
+      </c>
+      <c r="S2" t="s">
+        <v>82</v>
+      </c>
+      <c r="T2" t="s">
+        <v>76</v>
+      </c>
+      <c r="U2" t="s">
+        <v>77</v>
+      </c>
+      <c r="V2" t="s">
+        <v>78</v>
+      </c>
+      <c r="W2" t="s">
         <v>79</v>
-      </c>
-      <c r="R2" t="s">
-        <v>80</v>
-      </c>
-      <c r="S2" t="s">
-        <v>81</v>
-      </c>
-      <c r="T2" t="s">
-        <v>75</v>
-      </c>
-      <c r="U2" t="s">
-        <v>76</v>
-      </c>
-      <c r="V2" t="s">
-        <v>77</v>
-      </c>
-      <c r="W2" t="s">
-        <v>78</v>
       </c>
       <c r="X2">
         <v>22</v>
       </c>
       <c r="Y2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="Z2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="AA2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="AB2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="AC2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="AD2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="AE2">
         <v>2000</v>
@@ -969,69 +974,69 @@
         <v>12345</v>
       </c>
       <c r="AH2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="AI2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="AJ2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="AK2">
         <v>900</v>
       </c>
       <c r="AL2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="AM2" t="s">
+        <v>92</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>92</v>
+      </c>
+      <c r="AO2" t="s">
         <v>91</v>
-      </c>
-      <c r="AN2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AO2" t="s">
-        <v>90</v>
       </c>
       <c r="AP2">
         <v>2000</v>
       </c>
       <c r="AQ2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="AR2">
         <v>2010</v>
       </c>
       <c r="AS2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AT2" t="s">
+        <v>95</v>
+      </c>
+      <c r="AU2" t="s">
+        <v>96</v>
+      </c>
+      <c r="AV2" t="s">
         <v>94</v>
-      </c>
-      <c r="AU2" t="s">
-        <v>95</v>
-      </c>
-      <c r="AV2" t="s">
-        <v>93</v>
       </c>
       <c r="AW2">
         <v>2023</v>
       </c>
       <c r="AX2"/>
       <c r="AY2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="AZ2"/>
       <c r="BA2"/>
       <c r="BB2"/>
       <c r="BC2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="BD2"/>
       <c r="BE2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="BF2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="BG2"/>
       <c r="BH2"/>
@@ -1046,7 +1051,7 @@
       <c r="BQ2"/>
       <c r="BR2"/>
       <c r="BS2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>